<commit_message>
Advance Pivot and dynamic dashboard
</commit_message>
<xml_diff>
--- a/9. Conditional Formatting/Lecture_6_Formatting.xlsx
+++ b/9. Conditional Formatting/Lecture_6_Formatting.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3E7C3B-B800-494F-A030-2FA593D73B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="862" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="862" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw_Data" sheetId="26" r:id="rId1"/>
-    <sheet name="Worksheet" sheetId="28" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="29" r:id="rId2"/>
+    <sheet name="Worksheet" sheetId="28" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="EastAndWest">[1]INDEX!$D$91:$G$93,[1]INDEX!$D$96:$G$98</definedName>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
   <si>
     <t>Students</t>
   </si>
@@ -106,12 +108,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +183,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -346,7 +356,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -373,40 +383,63 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -430,54 +463,13 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -490,7 +482,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Welcome"/>
@@ -1328,17 +1320,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1396,7 +1390,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1425,7 +1419,7 @@
         <v>0.49333333333333335</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1454,7 +1448,7 @@
         <v>0.81333333333333335</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1483,7 +1477,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1512,7 +1506,7 @@
         <v>0.49833333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1541,7 +1535,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1570,7 +1564,7 @@
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1599,7 +1593,7 @@
         <v>0.73666666666666669</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1628,7 +1622,7 @@
         <v>0.80833333333333335</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1657,7 +1651,7 @@
         <v>0.67666666666666664</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1686,7 +1680,7 @@
         <v>0.64833333333333332</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1715,7 +1709,7 @@
         <v>0.66833333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1744,46 +1738,636 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201DE8FE-B6CB-4B95-A449-540CAC1EB5A6}">
+  <dimension ref="B2:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>99</v>
+      </c>
+      <c r="D3">
+        <v>83</v>
+      </c>
+      <c r="E3">
+        <v>85</v>
+      </c>
+      <c r="F3">
+        <v>82</v>
+      </c>
+      <c r="G3">
+        <v>69</v>
+      </c>
+      <c r="H3">
+        <v>92</v>
+      </c>
+      <c r="I3">
+        <v>510</v>
+      </c>
+      <c r="J3">
+        <v>0.85</v>
+      </c>
+      <c r="K3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>85</v>
+      </c>
+      <c r="D4">
+        <v>53</v>
+      </c>
+      <c r="E4">
+        <v>43</v>
+      </c>
+      <c r="F4">
+        <v>52</v>
+      </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>52</v>
+      </c>
+      <c r="I4">
+        <v>296</v>
+      </c>
+      <c r="J4">
+        <v>0.49333333333333335</v>
+      </c>
+      <c r="K4">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>85</v>
+      </c>
+      <c r="D5">
+        <v>80</v>
+      </c>
+      <c r="E5">
+        <v>79</v>
+      </c>
+      <c r="F5">
+        <v>79</v>
+      </c>
+      <c r="G5">
+        <v>74</v>
+      </c>
+      <c r="H5">
+        <v>91</v>
+      </c>
+      <c r="I5">
+        <v>488</v>
+      </c>
+      <c r="J5">
+        <v>0.81333333333333335</v>
+      </c>
+      <c r="K5">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>99</v>
+      </c>
+      <c r="E6">
+        <v>82</v>
+      </c>
+      <c r="F6">
+        <v>98</v>
+      </c>
+      <c r="G6">
+        <v>81</v>
+      </c>
+      <c r="H6">
+        <v>62</v>
+      </c>
+      <c r="I6">
+        <v>522</v>
+      </c>
+      <c r="J6">
+        <v>0.87</v>
+      </c>
+      <c r="K6">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>59</v>
+      </c>
+      <c r="G7">
+        <v>45</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7">
+        <v>299</v>
+      </c>
+      <c r="J7">
+        <v>0.49833333333333335</v>
+      </c>
+      <c r="K7">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <v>76</v>
+      </c>
+      <c r="E8">
+        <v>81</v>
+      </c>
+      <c r="F8">
+        <v>61</v>
+      </c>
+      <c r="G8">
+        <v>94</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+      <c r="I8">
+        <v>420</v>
+      </c>
+      <c r="J8">
+        <v>0.7</v>
+      </c>
+      <c r="K8">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>72</v>
+      </c>
+      <c r="D9">
+        <v>67</v>
+      </c>
+      <c r="E9">
+        <v>86</v>
+      </c>
+      <c r="F9">
+        <v>66</v>
+      </c>
+      <c r="G9">
+        <v>81</v>
+      </c>
+      <c r="H9">
+        <v>58</v>
+      </c>
+      <c r="I9">
+        <v>430</v>
+      </c>
+      <c r="J9">
+        <v>0.71666666666666667</v>
+      </c>
+      <c r="K9">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>82</v>
+      </c>
+      <c r="D10">
+        <v>63</v>
+      </c>
+      <c r="E10">
+        <v>72</v>
+      </c>
+      <c r="F10">
+        <v>80</v>
+      </c>
+      <c r="G10">
+        <v>53</v>
+      </c>
+      <c r="H10">
+        <v>92</v>
+      </c>
+      <c r="I10">
+        <v>442</v>
+      </c>
+      <c r="J10">
+        <v>0.73666666666666669</v>
+      </c>
+      <c r="K10">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>68</v>
+      </c>
+      <c r="D11">
+        <v>93</v>
+      </c>
+      <c r="E11">
+        <v>71</v>
+      </c>
+      <c r="F11">
+        <v>92</v>
+      </c>
+      <c r="G11">
+        <v>96</v>
+      </c>
+      <c r="H11">
+        <v>65</v>
+      </c>
+      <c r="I11">
+        <v>485</v>
+      </c>
+      <c r="J11">
+        <v>0.80833333333333335</v>
+      </c>
+      <c r="K11">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>59</v>
+      </c>
+      <c r="D12">
+        <v>89</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>57</v>
+      </c>
+      <c r="G12">
+        <v>31</v>
+      </c>
+      <c r="H12">
+        <v>75</v>
+      </c>
+      <c r="I12">
+        <v>406</v>
+      </c>
+      <c r="J12">
+        <v>0.67666666666666664</v>
+      </c>
+      <c r="K12">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>84</v>
+      </c>
+      <c r="D13">
+        <v>43</v>
+      </c>
+      <c r="E13">
+        <v>93</v>
+      </c>
+      <c r="F13">
+        <v>42</v>
+      </c>
+      <c r="G13">
+        <v>52</v>
+      </c>
+      <c r="H13">
+        <v>75</v>
+      </c>
+      <c r="I13">
+        <v>389</v>
+      </c>
+      <c r="J13">
+        <v>0.64833333333333332</v>
+      </c>
+      <c r="K13">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>94</v>
+      </c>
+      <c r="D14">
+        <v>72</v>
+      </c>
+      <c r="E14">
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>92</v>
+      </c>
+      <c r="G14">
+        <v>32</v>
+      </c>
+      <c r="H14">
+        <v>57</v>
+      </c>
+      <c r="I14">
+        <v>401</v>
+      </c>
+      <c r="J14">
+        <v>0.66833333333333333</v>
+      </c>
+      <c r="K14">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>78</v>
+      </c>
+      <c r="D15">
+        <v>73.166666666666671</v>
+      </c>
+      <c r="E15">
+        <v>72.583333333333329</v>
+      </c>
+      <c r="F15">
+        <v>71.666666666666671</v>
+      </c>
+      <c r="G15">
+        <v>59.916666666666664</v>
+      </c>
+      <c r="H15">
+        <v>68.666666666666671</v>
+      </c>
+      <c r="K15">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>488</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J3:J14">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThan">
+      <formula>0.681666667</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C15">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="lessThan">
+      <formula>72.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D14">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E14">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A05D626B-B187-48C2-BE03-6DEF69673A02}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F14">
+    <cfRule type="top10" dxfId="3" priority="5" percent="1" rank="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G14">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H14">
+    <cfRule type="duplicateValues" priority="3"/>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="35"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K20">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C7C08DA8-29B9-4962-8B27-EE2D2E83B2C0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A05D626B-B187-48C2-BE03-6DEF69673A02}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E3:E14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C7C08DA8-29B9-4962-8B27-EE2D2E83B2C0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K3:K20</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1812,7 +2396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
@@ -1837,11 +2421,11 @@
       <c r="I6" s="1">
         <v>510</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="10">
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
@@ -1866,11 +2450,11 @@
       <c r="I7" s="1">
         <v>296</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="10">
         <v>0.49333333333333335</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
@@ -1895,11 +2479,11 @@
       <c r="I8" s="1">
         <v>488</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="10">
         <v>0.81333333333333335</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1924,11 +2508,11 @@
       <c r="I9" s="1">
         <v>522</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="10">
         <v>0.87</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1953,11 +2537,11 @@
       <c r="I10" s="1">
         <v>299</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="10">
         <v>0.49833333333333335</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
@@ -1982,11 +2566,11 @@
       <c r="I11" s="1">
         <v>420</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="10">
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
@@ -2011,11 +2595,11 @@
       <c r="I12" s="1">
         <v>430</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="10">
         <v>0.71666666666666667</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
@@ -2040,11 +2624,11 @@
       <c r="I13" s="1">
         <v>442</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="10">
         <v>0.73666666666666669</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
@@ -2069,11 +2653,11 @@
       <c r="I14" s="1">
         <v>485</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="10">
         <v>0.80833333333333335</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
@@ -2098,11 +2682,11 @@
       <c r="I15" s="1">
         <v>406</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="10">
         <v>0.67666666666666664</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
@@ -2127,11 +2711,11 @@
       <c r="I16" s="1">
         <v>389</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="10">
         <v>0.64833333333333332</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
@@ -2156,30 +2740,30 @@
       <c r="I17" s="1">
         <v>401</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="10">
         <v>0.66833333333333333</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="11">
         <v>78</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="11">
         <v>73.166666666666671</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <v>72.583333333333329</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="11">
         <v>71.666666666666671</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="11">
         <v>59.916666666666664</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="11">
         <v>68.666666666666671</v>
       </c>
       <c r="I18" s="8"/>
@@ -2190,14 +2774,6 @@
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C6:H17">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
-      <formula>35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6:I17">
-    <cfRule type="top10" dxfId="0" priority="4" percent="1" rank="15"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C6:C17">
     <cfRule type="dataBar" priority="3">
       <dataBar>
@@ -2212,6 +2788,11 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C6:H17">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
+      <formula>35</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D6:D17">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -2223,6 +2804,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:I17">
+    <cfRule type="top10" dxfId="6" priority="4" percent="1" rank="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J17">
     <cfRule type="colorScale" priority="1">

</xml_diff>